<commit_message>
fixed ble_gatts_attr_t max_len = uint16_t. temperature & light value now uint16_t.
Signed-off-by: Temco_Heng <heng@temcocontrols.com>
</commit_message>
<xml_diff>
--- a/examples/nRF51-ble-bcast-mesh-0.8.7/docs/serial_interface.xlsx
+++ b/examples/nRF51-ble-bcast-mesh-0.8.7/docs/serial_interface.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trsn\Documents\SDK8\examples\nrf51-ble-bcast-mesh\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="180" windowWidth="17520" windowHeight="12645"/>
   </bookViews>
@@ -314,22 +309,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -337,14 +332,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -352,8 +347,15 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -613,40 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -660,6 +629,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -721,7 +723,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -756,7 +758,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -967,22 +969,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AQ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ45" sqref="AJ45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="37" customWidth="1"/>
+    <col min="1" max="1" width="3.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="46.75" customWidth="1"/>
+    <col min="4" max="4" width="7.75" style="37" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="42" width="2.85546875" style="2" customWidth="1"/>
-    <col min="43" max="43" width="49.42578125" customWidth="1"/>
+    <col min="6" max="42" width="2.875" style="2" customWidth="1"/>
+    <col min="43" max="43" width="49.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:43" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:43" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
         <v>48</v>
       </c>
@@ -1101,7 +1103,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1131,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1142,37 +1144,37 @@
       <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="47"/>
-      <c r="Y4" s="47"/>
-      <c r="Z4" s="47"/>
-      <c r="AA4" s="47"/>
-      <c r="AB4" s="47"/>
-      <c r="AC4" s="47"/>
-      <c r="AD4" s="47"/>
-      <c r="AE4" s="47"/>
-      <c r="AF4" s="47"/>
-      <c r="AG4" s="47"/>
-      <c r="AH4" s="48"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
+      <c r="U4" s="51"/>
+      <c r="V4" s="51"/>
+      <c r="W4" s="51"/>
+      <c r="X4" s="51"/>
+      <c r="Y4" s="51"/>
+      <c r="Z4" s="51"/>
+      <c r="AA4" s="51"/>
+      <c r="AB4" s="51"/>
+      <c r="AC4" s="51"/>
+      <c r="AD4" s="51"/>
+      <c r="AE4" s="51"/>
+      <c r="AF4" s="51"/>
+      <c r="AG4" s="51"/>
+      <c r="AH4" s="52"/>
       <c r="AI4" s="15"/>
       <c r="AJ4" s="16"/>
       <c r="AK4" s="16"/>
@@ -1182,7 +1184,7 @@
       <c r="AO4" s="16"/>
       <c r="AP4" s="16"/>
     </row>
-    <row r="5" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
         <v>50</v>
       </c>
@@ -1236,7 +1238,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -1249,18 +1251,18 @@
       <c r="E6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="43" t="s">
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="45"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="48"/>
       <c r="N6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1275,7 +1277,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1288,35 +1290,35 @@
       <c r="E7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42" t="s">
+      <c r="G7" s="41"/>
+      <c r="H7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="42"/>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="42"/>
-      <c r="Z7" s="42"/>
-      <c r="AA7" s="42"/>
-      <c r="AB7" s="42"/>
-      <c r="AC7" s="42"/>
-      <c r="AD7" s="42"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="41"/>
+      <c r="AD7" s="41"/>
       <c r="AE7" s="31"/>
       <c r="AF7" s="28"/>
       <c r="AG7" s="28"/>
@@ -1325,7 +1327,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
         <v>31</v>
       </c>
@@ -1338,15 +1340,15 @@
       <c r="E8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="42"/>
+      <c r="G8" s="41"/>
       <c r="AQ8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1359,15 +1361,15 @@
       <c r="E9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="42"/>
+      <c r="G9" s="41"/>
       <c r="AQ9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>59</v>
       </c>
@@ -1382,7 +1384,7 @@
       </c>
       <c r="F10" s="24"/>
     </row>
-    <row r="11" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>60</v>
       </c>
@@ -1397,7 +1399,7 @@
       </c>
       <c r="F11" s="24"/>
     </row>
-    <row r="12" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>68</v>
       </c>
@@ -1410,10 +1412,10 @@
       <c r="E12" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="42"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="25" t="s">
         <v>70</v>
       </c>
@@ -1430,7 +1432,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>69</v>
       </c>
@@ -1443,10 +1445,10 @@
       <c r="E13" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="41"/>
+      <c r="G13" s="55"/>
       <c r="H13" s="30" t="s">
         <v>70</v>
       </c>
@@ -1454,7 +1456,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>91</v>
       </c>
@@ -1467,41 +1469,41 @@
       <c r="E14" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
-      <c r="U14" s="42"/>
-      <c r="V14" s="42"/>
-      <c r="W14" s="42"/>
-      <c r="X14" s="42"/>
-      <c r="Y14" s="42"/>
-      <c r="Z14" s="42"/>
-      <c r="AA14" s="42"/>
-      <c r="AB14" s="42"/>
-      <c r="AC14" s="42"/>
-      <c r="AD14" s="42"/>
-    </row>
-    <row r="15" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="41"/>
+      <c r="AB14" s="41"/>
+      <c r="AC14" s="41"/>
+      <c r="AD14" s="41"/>
+    </row>
+    <row r="15" spans="2:43" x14ac:dyDescent="0.15">
       <c r="D15" s="14"/>
       <c r="E15" s="13"/>
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
     </row>
-    <row r="16" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1514,10 +1516,10 @@
       <c r="E16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -1546,7 +1548,7 @@
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -1587,7 +1589,7 @@
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>74</v>
       </c>
@@ -1630,7 +1632,7 @@
       <c r="AG18" s="6"/>
       <c r="AH18" s="6"/>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -1673,7 +1675,7 @@
       <c r="AG19" s="6"/>
       <c r="AH19" s="6"/>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>73</v>
       </c>
@@ -1716,7 +1718,7 @@
       <c r="AG20" s="6"/>
       <c r="AH20" s="6"/>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.15">
       <c r="D21" s="36"/>
       <c r="E21" s="11"/>
       <c r="F21" s="6"/>
@@ -1749,7 +1751,7 @@
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.15">
       <c r="D22" s="36"/>
       <c r="E22" s="11"/>
       <c r="F22" s="6"/>
@@ -1782,7 +1784,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.15">
       <c r="D23" s="36"/>
       <c r="E23" s="11"/>
       <c r="F23" s="6"/>
@@ -1815,7 +1817,7 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.15">
       <c r="D24" s="36"/>
       <c r="E24" s="11"/>
       <c r="F24" s="6"/>
@@ -1848,13 +1850,13 @@
       <c r="AG24" s="6"/>
       <c r="AH24" s="6"/>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.15">
       <c r="D25" s="36"/>
       <c r="E25" s="11"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
       <c r="D26" s="36"/>
       <c r="E26" s="11"/>
@@ -1869,7 +1871,7 @@
       <c r="AO26" s="6"/>
       <c r="AP26" s="6"/>
     </row>
-    <row r="27" spans="1:43" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:43" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="34" t="s">
         <v>49</v>
@@ -1887,7 +1889,7 @@
       <c r="AO27" s="18"/>
       <c r="AP27" s="18"/>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>11</v>
@@ -1929,7 +1931,7 @@
       <c r="AO28" s="16"/>
       <c r="AP28" s="16"/>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.15">
       <c r="B29" s="5" t="s">
         <v>54</v>
       </c>
@@ -1980,7 +1982,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.15">
       <c r="B30" s="5" t="s">
         <v>19</v>
       </c>
@@ -1991,37 +1993,37 @@
       <c r="E30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F30" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="47"/>
-      <c r="Q30" s="47"/>
-      <c r="R30" s="47"/>
-      <c r="S30" s="47"/>
-      <c r="T30" s="47"/>
-      <c r="U30" s="47"/>
-      <c r="V30" s="47"/>
-      <c r="W30" s="47"/>
-      <c r="X30" s="47"/>
-      <c r="Y30" s="47"/>
-      <c r="Z30" s="47"/>
-      <c r="AA30" s="47"/>
-      <c r="AB30" s="47"/>
-      <c r="AC30" s="47"/>
-      <c r="AD30" s="47"/>
-      <c r="AE30" s="47"/>
-      <c r="AF30" s="47"/>
-      <c r="AG30" s="47"/>
-      <c r="AH30" s="48"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
+      <c r="T30" s="51"/>
+      <c r="U30" s="51"/>
+      <c r="V30" s="51"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
+      <c r="Y30" s="51"/>
+      <c r="Z30" s="51"/>
+      <c r="AA30" s="51"/>
+      <c r="AB30" s="51"/>
+      <c r="AC30" s="51"/>
+      <c r="AD30" s="51"/>
+      <c r="AE30" s="51"/>
+      <c r="AF30" s="51"/>
+      <c r="AG30" s="51"/>
+      <c r="AH30" s="52"/>
       <c r="AI30" s="28"/>
       <c r="AK30"/>
       <c r="AL30"/>
@@ -2030,7 +2032,7 @@
       <c r="AO30"/>
       <c r="AP30"/>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>12</v>
       </c>
@@ -2049,33 +2051,33 @@
       <c r="G31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="43" t="s">
+      <c r="H31" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
-      <c r="P31" s="44"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="44"/>
-      <c r="S31" s="44"/>
-      <c r="T31" s="44"/>
-      <c r="U31" s="44"/>
-      <c r="V31" s="44"/>
-      <c r="W31" s="44"/>
-      <c r="X31" s="44"/>
-      <c r="Y31" s="44"/>
-      <c r="Z31" s="44"/>
-      <c r="AA31" s="44"/>
-      <c r="AB31" s="44"/>
-      <c r="AC31" s="44"/>
-      <c r="AD31" s="44"/>
-      <c r="AE31" s="44"/>
-      <c r="AF31" s="45"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="49"/>
+      <c r="U31" s="49"/>
+      <c r="V31" s="49"/>
+      <c r="W31" s="49"/>
+      <c r="X31" s="49"/>
+      <c r="Y31" s="49"/>
+      <c r="Z31" s="49"/>
+      <c r="AA31" s="49"/>
+      <c r="AB31" s="49"/>
+      <c r="AC31" s="49"/>
+      <c r="AD31" s="49"/>
+      <c r="AE31" s="49"/>
+      <c r="AF31" s="48"/>
       <c r="AG31" s="28"/>
       <c r="AH31" s="28"/>
       <c r="AI31" s="28"/>
@@ -2089,7 +2091,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.15">
       <c r="C32" t="s">
         <v>69</v>
       </c>
@@ -2099,10 +2101,10 @@
       <c r="E32" s="12"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="49" t="s">
+      <c r="H32" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="50"/>
+      <c r="I32" s="57"/>
       <c r="J32" s="33" t="s">
         <v>70</v>
       </c>
@@ -2124,44 +2126,44 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:43" x14ac:dyDescent="0.15">
       <c r="C33" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H33" s="42" t="s">
+      <c r="H33" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I33" s="42"/>
-      <c r="J33" s="43" t="s">
+      <c r="I33" s="41"/>
+      <c r="J33" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="K33" s="44"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="44"/>
-      <c r="N33" s="44"/>
-      <c r="O33" s="44"/>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="44"/>
-      <c r="T33" s="44"/>
-      <c r="U33" s="44"/>
-      <c r="V33" s="44"/>
-      <c r="W33" s="44"/>
-      <c r="X33" s="44"/>
-      <c r="Y33" s="44"/>
-      <c r="Z33" s="44"/>
-      <c r="AA33" s="44"/>
-      <c r="AB33" s="44"/>
-      <c r="AC33" s="44"/>
-      <c r="AD33" s="44"/>
-      <c r="AE33" s="44"/>
-      <c r="AF33" s="45"/>
-    </row>
-    <row r="34" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="49"/>
+      <c r="U33" s="49"/>
+      <c r="V33" s="49"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="49"/>
+      <c r="Y33" s="49"/>
+      <c r="Z33" s="49"/>
+      <c r="AA33" s="49"/>
+      <c r="AB33" s="49"/>
+      <c r="AC33" s="49"/>
+      <c r="AD33" s="49"/>
+      <c r="AE33" s="49"/>
+      <c r="AF33" s="48"/>
+    </row>
+    <row r="34" spans="2:43" x14ac:dyDescent="0.15">
       <c r="C34" t="s">
         <v>32</v>
       </c>
@@ -2181,21 +2183,21 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:43" x14ac:dyDescent="0.15">
       <c r="C35" t="s">
         <v>74</v>
       </c>
       <c r="D35" s="9">
         <v>7</v>
       </c>
-      <c r="H35" s="42" t="s">
+      <c r="H35" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="42"/>
-    </row>
-    <row r="36" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+    </row>
+    <row r="36" spans="2:43" x14ac:dyDescent="0.15">
       <c r="C36" t="s">
         <v>35</v>
       </c>
@@ -2206,36 +2208,36 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:43" x14ac:dyDescent="0.15">
       <c r="C37" t="s">
         <v>73</v>
       </c>
       <c r="D37" s="9">
         <v>7</v>
       </c>
-      <c r="H37" s="42" t="s">
+      <c r="H37" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
-      <c r="K37" s="42"/>
-    </row>
-    <row r="38" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="41"/>
+    </row>
+    <row r="38" spans="2:43" x14ac:dyDescent="0.15">
       <c r="C38" t="s">
         <v>91</v>
       </c>
       <c r="D38" s="9">
         <v>5</v>
       </c>
-      <c r="H38" s="42" t="s">
+      <c r="H38" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I38" s="42"/>
+      <c r="I38" s="41"/>
       <c r="AQ38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
         <v>13</v>
       </c>
@@ -2245,40 +2247,40 @@
       <c r="E39" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="42" t="s">
+      <c r="F39" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="42"/>
-      <c r="H39" s="43" t="s">
+      <c r="G39" s="41"/>
+      <c r="H39" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="44"/>
-      <c r="N39" s="44"/>
-      <c r="O39" s="44"/>
-      <c r="P39" s="44"/>
-      <c r="Q39" s="44"/>
-      <c r="R39" s="44"/>
-      <c r="S39" s="44"/>
-      <c r="T39" s="44"/>
-      <c r="U39" s="44"/>
-      <c r="V39" s="44"/>
-      <c r="W39" s="44"/>
-      <c r="X39" s="44"/>
-      <c r="Y39" s="44"/>
-      <c r="Z39" s="44"/>
-      <c r="AA39" s="44"/>
-      <c r="AB39" s="44"/>
-      <c r="AC39" s="44"/>
-      <c r="AD39" s="45"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="49"/>
+      <c r="U39" s="49"/>
+      <c r="V39" s="49"/>
+      <c r="W39" s="49"/>
+      <c r="X39" s="49"/>
+      <c r="Y39" s="49"/>
+      <c r="Z39" s="49"/>
+      <c r="AA39" s="49"/>
+      <c r="AB39" s="49"/>
+      <c r="AC39" s="49"/>
+      <c r="AD39" s="48"/>
       <c r="AQ39" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>14</v>
       </c>
@@ -2288,40 +2290,40 @@
       <c r="E40" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="42" t="s">
+      <c r="F40" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="42"/>
-      <c r="H40" s="43" t="s">
+      <c r="G40" s="41"/>
+      <c r="H40" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="44"/>
-      <c r="N40" s="44"/>
-      <c r="O40" s="44"/>
-      <c r="P40" s="44"/>
-      <c r="Q40" s="44"/>
-      <c r="R40" s="44"/>
-      <c r="S40" s="44"/>
-      <c r="T40" s="44"/>
-      <c r="U40" s="44"/>
-      <c r="V40" s="44"/>
-      <c r="W40" s="44"/>
-      <c r="X40" s="44"/>
-      <c r="Y40" s="44"/>
-      <c r="Z40" s="44"/>
-      <c r="AA40" s="44"/>
-      <c r="AB40" s="44"/>
-      <c r="AC40" s="44"/>
-      <c r="AD40" s="45"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="49"/>
+      <c r="U40" s="49"/>
+      <c r="V40" s="49"/>
+      <c r="W40" s="49"/>
+      <c r="X40" s="49"/>
+      <c r="Y40" s="49"/>
+      <c r="Z40" s="49"/>
+      <c r="AA40" s="49"/>
+      <c r="AB40" s="49"/>
+      <c r="AC40" s="49"/>
+      <c r="AD40" s="48"/>
       <c r="AQ40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
         <v>15</v>
       </c>
@@ -2331,40 +2333,40 @@
       <c r="E41" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="43" t="s">
+      <c r="F41" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="45"/>
-      <c r="H41" s="43" t="s">
+      <c r="G41" s="48"/>
+      <c r="H41" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I41" s="44"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="44"/>
-      <c r="M41" s="44"/>
-      <c r="N41" s="44"/>
-      <c r="O41" s="44"/>
-      <c r="P41" s="44"/>
-      <c r="Q41" s="44"/>
-      <c r="R41" s="44"/>
-      <c r="S41" s="44"/>
-      <c r="T41" s="44"/>
-      <c r="U41" s="44"/>
-      <c r="V41" s="44"/>
-      <c r="W41" s="44"/>
-      <c r="X41" s="44"/>
-      <c r="Y41" s="44"/>
-      <c r="Z41" s="44"/>
-      <c r="AA41" s="44"/>
-      <c r="AB41" s="44"/>
-      <c r="AC41" s="44"/>
-      <c r="AD41" s="45"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="49"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="49"/>
+      <c r="U41" s="49"/>
+      <c r="V41" s="49"/>
+      <c r="W41" s="49"/>
+      <c r="X41" s="49"/>
+      <c r="Y41" s="49"/>
+      <c r="Z41" s="49"/>
+      <c r="AA41" s="49"/>
+      <c r="AB41" s="49"/>
+      <c r="AC41" s="49"/>
+      <c r="AD41" s="48"/>
       <c r="AQ41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="2:43" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:43" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
         <v>89</v>
       </c>
@@ -2374,80 +2376,66 @@
       <c r="E42" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="43" t="s">
+      <c r="F42" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="45"/>
-      <c r="H42" s="43" t="s">
+      <c r="G42" s="48"/>
+      <c r="H42" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44"/>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="44"/>
-      <c r="S42" s="44"/>
-      <c r="T42" s="44"/>
-      <c r="U42" s="44"/>
-      <c r="V42" s="44"/>
-      <c r="W42" s="44"/>
-      <c r="X42" s="44"/>
-      <c r="Y42" s="44"/>
-      <c r="Z42" s="44"/>
-      <c r="AA42" s="44"/>
-      <c r="AB42" s="44"/>
-      <c r="AC42" s="44"/>
-      <c r="AD42" s="45"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="49"/>
+      <c r="U42" s="49"/>
+      <c r="V42" s="49"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="49"/>
+      <c r="Y42" s="49"/>
+      <c r="Z42" s="49"/>
+      <c r="AA42" s="49"/>
+      <c r="AB42" s="49"/>
+      <c r="AC42" s="49"/>
+      <c r="AD42" s="48"/>
       <c r="AQ42" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B44" s="53" t="s">
+    <row r="44" spans="2:43" x14ac:dyDescent="0.15">
+      <c r="B44" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="54"/>
-      <c r="D44" s="55"/>
-    </row>
-    <row r="45" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B45" s="56" t="s">
+      <c r="C44" s="43"/>
+      <c r="D44" s="44"/>
+    </row>
+    <row r="45" spans="2:43" x14ac:dyDescent="0.15">
+      <c r="B45" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="57"/>
+      <c r="C45" s="46"/>
       <c r="D45" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B46" s="56" t="s">
+    <row r="46" spans="2:43" x14ac:dyDescent="0.15">
+      <c r="B46" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="57"/>
+      <c r="C46" s="46"/>
       <c r="D46" s="9" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:AD42"/>
-    <mergeCell ref="F4:AH4"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H7:AD7"/>
-    <mergeCell ref="J6:M6"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="H41:AD41"/>
@@ -2464,7 +2452,22 @@
     <mergeCell ref="H31:AF31"/>
     <mergeCell ref="F14:AD14"/>
     <mergeCell ref="H38:I38"/>
+    <mergeCell ref="F4:AH4"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H7:AD7"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:AD42"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2476,8 +2479,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2488,8 +2492,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>